<commit_message>
frequencias relativas (geral, relevante)
</commit_message>
<xml_diff>
--- a/pokemon_classificado.xlsx
+++ b/pokemon_classificado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fuque\Desktop\Drive\INSPER\ciencia_dos_dados\projeto2_Cdados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E916E4-1144-4967-A78B-BA0F00B88B3E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5C65AA-0153-4FE9-9929-A860C93BF177}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2113,7 +2113,7 @@
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>